<commit_message>
Starting to add positional rankings
</commit_message>
<xml_diff>
--- a/LineupGenerator/Data/DummyData.xlsx
+++ b/LineupGenerator/Data/DummyData.xlsx
@@ -438,7 +438,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -485,34 +487,34 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -523,31 +525,31 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -555,34 +557,34 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -590,34 +592,34 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -625,34 +627,34 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -660,34 +662,34 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -695,34 +697,34 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -730,34 +732,34 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -765,34 +767,34 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -800,31 +802,31 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -835,34 +837,34 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First attempt at full generated lineup
</commit_message>
<xml_diff>
--- a/LineupGenerator/Data/DummyData.xlsx
+++ b/LineupGenerator/Data/DummyData.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Andy</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Purdy</t>
   </si>
   <si>
-    <t>BenchWarmer</t>
-  </si>
-  <si>
     <t>FirstBase</t>
   </si>
   <si>
@@ -85,13 +82,19 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Bench2</t>
+  </si>
+  <si>
+    <t>Bench1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,7 +185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -234,7 +237,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -428,61 +431,61 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -517,7 +520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -552,7 +555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -587,7 +590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -622,7 +625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -657,7 +660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -692,7 +695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -727,7 +730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -747,7 +750,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>5</v>
@@ -762,7 +765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -797,7 +800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -832,39 +835,74 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K12">
-        <v>4</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>